<commit_message>
#85: Confirms full runs across templates
</commit_message>
<xml_diff>
--- a/paper_slides/tables/skeletons/latex_test_longtable_extremecase.xlsx
+++ b/paper_slides/tables/skeletons/latex_test_longtable_extremecase.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11028"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11110"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sameernair-desai/Desktop/InstRes/SIEPR_RA/template/paper_slides/code/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sameernair-desai/Desktop/InstRes/SIEPR_RA/template/paper_slides/tables/skeletons/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A4ABDC7-957F-974D-BA0F-28B558FAF72D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A4CBE59-C3F2-104D-AA83-DB270237DE2C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31360" yWindow="7700" windowWidth="37540" windowHeight="17440" activeTab="1" xr2:uid="{B390F614-ADA4-ED45-B7F9-CAB4E813F00D}"/>
+    <workbookView xWindow="31300" yWindow="2720" windowWidth="37540" windowHeight="17440" xr2:uid="{B390F614-ADA4-ED45-B7F9-CAB4E813F00D}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
-    <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="Scalars" sheetId="1" r:id="rId1"/>
+    <sheet name="Table" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,40 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="24">
-  <si>
-    <t>Strong</t>
-  </si>
-  <si>
-    <t>Democrat</t>
-  </si>
-  <si>
-    <t>Independent</t>
-  </si>
-  <si>
-    <t>Republican</t>
-  </si>
-  <si>
-    <t>Seen Banner</t>
-  </si>
-  <si>
-    <t>Table S2: Experimental Summary Statistics by Political Leaning</t>
-  </si>
-  <si>
-    <t>Clicked Banner</t>
-  </si>
-  <si>
-    <t>Consented</t>
-  </si>
-  <si>
-    <t>Completed Baseline Survey</t>
-  </si>
-  <si>
-    <t>Completed Endline Survey</t>
-  </si>
-  <si>
-    <t>Total Attrition Rate</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="13">
   <si>
     <r>
       <rPr>
@@ -176,7 +143,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -187,28 +154,8 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
       <top/>
       <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="medium">
         <color indexed="64"/>
       </bottom>
       <diagonal/>
@@ -295,49 +242,41 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="3" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -655,10 +594,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D491D851-0BDE-2243-9EB9-D84ECB9E783F}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F19" sqref="E19:F19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -671,201 +610,77 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
-        <v>5</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
+      <c r="A1" s="14"/>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="19"/>
-      <c r="D2" s="19"/>
-      <c r="E2" s="19"/>
-      <c r="F2" s="19"/>
+      <c r="A2" s="15"/>
+      <c r="B2" s="15"/>
+      <c r="C2" s="15"/>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="1"/>
-      <c r="B3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>0</v>
-      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2"/>
+      <c r="E3" s="2"/>
+      <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A4" s="2"/>
-      <c r="B4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4" t="s">
-        <v>3</v>
-      </c>
+      <c r="B4" s="2"/>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="2"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" s="6">
-        <v>3436123</v>
-      </c>
-      <c r="C5" s="6">
-        <v>5245121</v>
-      </c>
-      <c r="D5" s="6">
-        <v>850321</v>
-      </c>
-      <c r="E5" s="6">
-        <v>3506722</v>
-      </c>
-      <c r="F5" s="6">
-        <v>1519232</v>
-      </c>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>6</v>
-      </c>
-      <c r="B6" s="6">
-        <v>5328294534985430</v>
-      </c>
-      <c r="C6" s="6">
-        <f t="shared" ref="C6:F6" si="0">C5*0.85</f>
-        <v>4458352.8499999996</v>
-      </c>
-      <c r="D6" s="6">
-        <f t="shared" si="0"/>
-        <v>722772.85</v>
-      </c>
-      <c r="E6" s="6">
-        <f t="shared" si="0"/>
-        <v>2980713.6999999997</v>
-      </c>
-      <c r="F6" s="6">
-        <f t="shared" si="0"/>
-        <v>1291347.2</v>
-      </c>
+      <c r="B6" s="11"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>7</v>
-      </c>
-      <c r="B7" s="6">
-        <f>0.23*B6</f>
-        <v>1225507743046649</v>
-      </c>
-      <c r="C7" s="6">
-        <f t="shared" ref="C7:F7" si="1">0.23*C6</f>
-        <v>1025421.1555</v>
-      </c>
-      <c r="D7" s="6">
-        <f t="shared" si="1"/>
-        <v>166237.7555</v>
-      </c>
-      <c r="E7" s="6">
-        <f t="shared" si="1"/>
-        <v>685564.15099999995</v>
-      </c>
-      <c r="F7" s="6">
-        <f t="shared" si="1"/>
-        <v>297009.85600000003</v>
-      </c>
+      <c r="B7" s="11"/>
+      <c r="C7" s="11"/>
+      <c r="D7" s="11"/>
+      <c r="E7" s="11"/>
+      <c r="F7" s="11"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>8</v>
-      </c>
-      <c r="B8" s="6">
-        <f>0.45*B7</f>
-        <v>551478484370992.06</v>
-      </c>
-      <c r="C8" s="6">
-        <f t="shared" ref="C8:F8" si="2">0.45*C7</f>
-        <v>461439.519975</v>
-      </c>
-      <c r="D8" s="6">
-        <f t="shared" si="2"/>
-        <v>74806.989975000004</v>
-      </c>
-      <c r="E8" s="6">
-        <f t="shared" si="2"/>
-        <v>308503.86794999999</v>
-      </c>
-      <c r="F8" s="6">
-        <f t="shared" si="2"/>
-        <v>133654.43520000001</v>
-      </c>
+      <c r="B8" s="11"/>
+      <c r="C8" s="11"/>
+      <c r="D8" s="11"/>
+      <c r="E8" s="11"/>
+      <c r="F8" s="11"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A9" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="B9" s="7">
-        <f>0.12*B8</f>
-        <v>66177418124519.047</v>
-      </c>
-      <c r="C9" s="7">
-        <f t="shared" ref="C9:F9" si="3">0.12*C8</f>
-        <v>55372.742397000002</v>
-      </c>
-      <c r="D9" s="7">
-        <f t="shared" si="3"/>
-        <v>8976.8387970000003</v>
-      </c>
-      <c r="E9" s="7">
-        <f t="shared" si="3"/>
-        <v>37020.464153999994</v>
-      </c>
-      <c r="F9" s="7">
-        <f t="shared" si="3"/>
-        <v>16038.532224</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
-        <v>10</v>
-      </c>
-      <c r="B10" s="8">
-        <f>(B5-B9)/B5</f>
-        <v>-19259326.481734224</v>
-      </c>
-      <c r="C10" s="8">
-        <f t="shared" ref="C10:F10" si="4">(C5-C9)/C5</f>
-        <v>0.98944299999999996</v>
-      </c>
-      <c r="D10" s="8">
-        <f t="shared" si="4"/>
-        <v>0.98944299999999996</v>
-      </c>
-      <c r="E10" s="8">
-        <f t="shared" si="4"/>
-        <v>0.98944300000000007</v>
-      </c>
-      <c r="F10" s="8">
-        <f t="shared" si="4"/>
-        <v>0.98944300000000007</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
+      <c r="B9" s="11"/>
+      <c r="C9" s="11"/>
+      <c r="D9" s="11"/>
+      <c r="E9" s="11"/>
+      <c r="F9" s="11"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="12"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="13"/>
+      <c r="D10" s="13"/>
+      <c r="E10" s="13"/>
+      <c r="F10" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -881,8 +696,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1749E75-5A09-FA4F-91F7-E36EDA50930F}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -897,385 +712,385 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="18" t="s">
-        <v>23</v>
-      </c>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
+      <c r="A1" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B1" s="14"/>
+      <c r="C1" s="14"/>
+      <c r="D1" s="14"/>
+      <c r="E1" s="14"/>
+      <c r="F1" s="14"/>
+      <c r="G1" s="14"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="14"/>
-      <c r="B3" s="10" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="10" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="10" t="s">
-        <v>21</v>
-      </c>
-      <c r="G3" s="11" t="s">
-        <v>22</v>
+      <c r="A3" s="7"/>
+      <c r="B3" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" s="4" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B4" s="9">
+      <c r="A4" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B4" s="2">
         <v>3436123</v>
       </c>
-      <c r="C4" s="9">
+      <c r="C4" s="2">
         <v>2920704.55</v>
       </c>
-      <c r="D4" s="9">
+      <c r="D4" s="2">
         <v>671762.04649999994</v>
       </c>
-      <c r="E4" s="9">
+      <c r="E4" s="2">
         <v>302292.92092499998</v>
       </c>
-      <c r="F4" s="9">
+      <c r="F4" s="2">
         <v>36275.150511</v>
       </c>
-      <c r="G4" s="12">
+      <c r="G4" s="5">
         <v>0.98944300000000007</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" s="9">
+      <c r="A5" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="2">
         <v>5245121</v>
       </c>
-      <c r="C5" s="9">
+      <c r="C5" s="2">
         <v>4458352.8499999996</v>
       </c>
-      <c r="D5" s="9">
+      <c r="D5" s="2">
         <v>1025421.1555</v>
       </c>
-      <c r="E5" s="9">
+      <c r="E5" s="2">
         <v>461439.519975</v>
       </c>
-      <c r="F5" s="9">
+      <c r="F5" s="2">
         <v>55372.742397000002</v>
       </c>
-      <c r="G5" s="12">
+      <c r="G5" s="5">
         <v>0.98944299999999996</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" s="9">
+      <c r="A6" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B6" s="2">
         <v>850321</v>
       </c>
-      <c r="C6" s="9">
+      <c r="C6" s="2">
         <v>722772.85</v>
       </c>
-      <c r="D6" s="9">
+      <c r="D6" s="2">
         <v>166237.7555</v>
       </c>
-      <c r="E6" s="9">
+      <c r="E6" s="2">
         <v>74806.989975000004</v>
       </c>
-      <c r="F6" s="9">
+      <c r="F6" s="2">
         <v>8976.8387970000003</v>
       </c>
-      <c r="G6" s="12">
+      <c r="G6" s="5">
         <v>0.98944299999999996</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B7" s="9">
+      <c r="A7" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B7" s="2">
         <v>3506722</v>
       </c>
-      <c r="C7" s="9">
+      <c r="C7" s="2">
         <v>2980713.6999999997</v>
       </c>
-      <c r="D7" s="9">
+      <c r="D7" s="2">
         <v>685564.15099999995</v>
       </c>
-      <c r="E7" s="9">
+      <c r="E7" s="2">
         <v>308503.86794999999</v>
       </c>
-      <c r="F7" s="9">
+      <c r="F7" s="2">
         <v>37020.464153999994</v>
       </c>
-      <c r="G7" s="12">
+      <c r="G7" s="5">
         <v>0.98944300000000007</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A8" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" s="9">
+      <c r="A8" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" s="2">
         <v>1519232</v>
       </c>
-      <c r="C8" s="9">
+      <c r="C8" s="2">
         <v>1291347.2</v>
       </c>
-      <c r="D8" s="9">
+      <c r="D8" s="2">
         <v>297009.85600000003</v>
       </c>
-      <c r="E8" s="9">
+      <c r="E8" s="2">
         <v>133654.43520000001</v>
       </c>
-      <c r="F8" s="9">
+      <c r="F8" s="2">
         <v>16038.532224</v>
       </c>
-      <c r="G8" s="12">
+      <c r="G8" s="5">
         <v>0.98944300000000007</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A9" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B9" s="9">
+      <c r="A9" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B9" s="2">
         <v>3436123</v>
       </c>
-      <c r="C9" s="9">
+      <c r="C9" s="2">
         <v>2920704.55</v>
       </c>
-      <c r="D9" s="9">
+      <c r="D9" s="2">
         <v>671762.04649999994</v>
       </c>
-      <c r="E9" s="9">
+      <c r="E9" s="2">
         <v>302292.92092499998</v>
       </c>
-      <c r="F9" s="9">
+      <c r="F9" s="2">
         <v>36275.150511</v>
       </c>
-      <c r="G9" s="12">
+      <c r="G9" s="5">
         <v>0.98944300000000007</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A10" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="B10" s="9">
+      <c r="A10" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B10" s="2">
         <v>5245121</v>
       </c>
-      <c r="C10" s="9">
+      <c r="C10" s="2">
         <v>4458352.8499999996</v>
       </c>
-      <c r="D10" s="9">
+      <c r="D10" s="2">
         <v>1025421.1555</v>
       </c>
-      <c r="E10" s="9">
+      <c r="E10" s="2">
         <v>461439.519975</v>
       </c>
-      <c r="F10" s="9">
+      <c r="F10" s="2">
         <v>55372.742397000002</v>
       </c>
-      <c r="G10" s="12">
+      <c r="G10" s="5">
         <v>0.98944299999999996</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A11" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B11" s="9">
+      <c r="A11" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B11" s="2">
         <v>850321</v>
       </c>
-      <c r="C11" s="9">
+      <c r="C11" s="2">
         <v>722772.85</v>
       </c>
-      <c r="D11" s="9">
+      <c r="D11" s="2">
         <v>166237.7555</v>
       </c>
-      <c r="E11" s="9">
+      <c r="E11" s="2">
         <v>74806.989975000004</v>
       </c>
-      <c r="F11" s="9">
+      <c r="F11" s="2">
         <v>8976.8387970000003</v>
       </c>
-      <c r="G11" s="12">
+      <c r="G11" s="5">
         <v>0.98944299999999996</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A12" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B12" s="9">
+      <c r="A12" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B12" s="2">
         <v>3506722</v>
       </c>
-      <c r="C12" s="9">
+      <c r="C12" s="2">
         <v>2980713.6999999997</v>
       </c>
-      <c r="D12" s="9">
+      <c r="D12" s="2">
         <v>685564.15099999995</v>
       </c>
-      <c r="E12" s="9">
+      <c r="E12" s="2">
         <v>308503.86794999999</v>
       </c>
-      <c r="F12" s="9">
+      <c r="F12" s="2">
         <v>37020.464153999994</v>
       </c>
-      <c r="G12" s="12">
+      <c r="G12" s="5">
         <v>0.98944300000000007</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A13" s="16" t="s">
-        <v>16</v>
-      </c>
-      <c r="B13" s="9">
+      <c r="A13" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B13" s="2">
         <v>1519232</v>
       </c>
-      <c r="C13" s="9">
+      <c r="C13" s="2">
         <v>1291347.2</v>
       </c>
-      <c r="D13" s="9">
+      <c r="D13" s="2">
         <v>297009.85600000003</v>
       </c>
-      <c r="E13" s="9">
+      <c r="E13" s="2">
         <v>133654.43520000001</v>
       </c>
-      <c r="F13" s="9">
+      <c r="F13" s="2">
         <v>16038.532224</v>
       </c>
-      <c r="G13" s="12">
+      <c r="G13" s="5">
         <v>0.98944300000000007</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A14" s="15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B14" s="9">
+      <c r="A14" s="8" t="s">
+        <v>1</v>
+      </c>
+      <c r="B14" s="2">
         <v>3436123</v>
       </c>
-      <c r="C14" s="9">
+      <c r="C14" s="2">
         <v>2920704.55</v>
       </c>
-      <c r="D14" s="9">
+      <c r="D14" s="2">
         <v>671762.04649999994</v>
       </c>
-      <c r="E14" s="9">
+      <c r="E14" s="2">
         <v>302292.92092499998</v>
       </c>
-      <c r="F14" s="9">
+      <c r="F14" s="2">
         <v>36275.150511</v>
       </c>
-      <c r="G14" s="12">
+      <c r="G14" s="5">
         <v>0.98944300000000007</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A15" s="16" t="s">
-        <v>13</v>
-      </c>
-      <c r="B15" s="9">
+      <c r="A15" s="9" t="s">
+        <v>2</v>
+      </c>
+      <c r="B15" s="2">
         <v>5245121</v>
       </c>
-      <c r="C15" s="9">
+      <c r="C15" s="2">
         <v>4458352.8499999996</v>
       </c>
-      <c r="D15" s="9">
+      <c r="D15" s="2">
         <v>1025421.1555</v>
       </c>
-      <c r="E15" s="9">
+      <c r="E15" s="2">
         <v>461439.519975</v>
       </c>
-      <c r="F15" s="9">
+      <c r="F15" s="2">
         <v>55372.742397000002</v>
       </c>
-      <c r="G15" s="12">
+      <c r="G15" s="5">
         <v>0.98944299999999996</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A16" s="16" t="s">
-        <v>14</v>
-      </c>
-      <c r="B16" s="9">
+      <c r="A16" s="9" t="s">
+        <v>3</v>
+      </c>
+      <c r="B16" s="2">
         <v>850321</v>
       </c>
-      <c r="C16" s="9">
+      <c r="C16" s="2">
         <v>722772.85</v>
       </c>
-      <c r="D16" s="9">
+      <c r="D16" s="2">
         <v>166237.7555</v>
       </c>
-      <c r="E16" s="9">
+      <c r="E16" s="2">
         <v>74806.989975000004</v>
       </c>
-      <c r="F16" s="9">
+      <c r="F16" s="2">
         <v>8976.8387970000003</v>
       </c>
-      <c r="G16" s="12">
+      <c r="G16" s="5">
         <v>0.98944299999999996</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A17" s="16" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="9">
+      <c r="A17" s="9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B17" s="2">
         <v>3506722</v>
       </c>
-      <c r="C17" s="9">
+      <c r="C17" s="2">
         <v>2980713.6999999997</v>
       </c>
-      <c r="D17" s="9">
+      <c r="D17" s="2">
         <v>685564.15099999995</v>
       </c>
-      <c r="E17" s="9">
+      <c r="E17" s="2">
         <v>308503.86794999999</v>
       </c>
-      <c r="F17" s="9">
+      <c r="F17" s="2">
         <v>37020.464153999994</v>
       </c>
-      <c r="G17" s="12">
+      <c r="G17" s="5">
         <v>0.98944300000000007</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A18" s="17" t="s">
-        <v>16</v>
-      </c>
-      <c r="B18" s="4">
+      <c r="A18" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B18" s="1">
         <v>1519232</v>
       </c>
-      <c r="C18" s="4">
+      <c r="C18" s="1">
         <v>1291347.2</v>
       </c>
-      <c r="D18" s="4">
+      <c r="D18" s="1">
         <v>297009.85600000003</v>
       </c>
-      <c r="E18" s="4">
+      <c r="E18" s="1">
         <v>133654.43520000001</v>
       </c>
-      <c r="F18" s="4">
+      <c r="F18" s="1">
         <v>16038.532224</v>
       </c>
-      <c r="G18" s="13">
+      <c r="G18" s="6">
         <v>0.98944300000000007</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
-        <v>11</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>